<commit_message>
Teste envio para VPS
</commit_message>
<xml_diff>
--- a/Esboços.xlsx
+++ b/Esboços.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Documents\GitHub\controleGastos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F489EC8C-283F-4AEE-83FA-64F642263E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D73CDD-FAC3-43B6-8E8D-2D93B46C1719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1231ACE8-AA2C-4706-98BD-BE4A7629A409}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1231ACE8-AA2C-4706-98BD-BE4A7629A409}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Pagamento" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
   <si>
     <t>Coluna</t>
   </si>
@@ -122,12 +122,6 @@
     <t>codigoMesAnoPagamento</t>
   </si>
   <si>
-    <t>numeroMesPagamento</t>
-  </si>
-  <si>
-    <t>numeroAnoPagamento</t>
-  </si>
-  <si>
     <t>codigoValorPagamento</t>
   </si>
   <si>
@@ -168,6 +162,18 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>dataInclusao</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>mesPagamento</t>
+  </si>
+  <si>
+    <t>anoPagamento</t>
   </si>
 </sst>
 </file>
@@ -665,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620D6242-9631-479A-A03F-898E9050F323}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +700,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -702,7 +708,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -713,10 +719,10 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1014,7 +1020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED154509-A5D0-4461-81C0-A41EDF3DE266}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1039,7 +1047,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -1047,7 +1055,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -1063,7 +1071,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1071,7 +1079,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -1079,10 +1087,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1096,30 +1104,30 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>37</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1150,25 +1158,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
         <v>8</v>
@@ -1182,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1212,7 +1220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8426C7D4-78BD-49CE-B35F-B03096772C1F}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1233,7 +1243,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -1249,7 +1259,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1266,7 +1276,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1274,16 +1284,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>